<commit_message>
review expected results 400
</commit_message>
<xml_diff>
--- a/excel/customers-risksanalysis-v1.xlsx
+++ b/excel/customers-risksanalysis-v1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="159">
   <si>
     <t>Subject</t>
   </si>
@@ -490,17 +490,17 @@
   "apiVersion": "1;2020-06-11",
   "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
   "error": {
-    "httpCode": "401",
-    "errorCode": "API-RISKSANALYSIS-401",
-    "message": "Unauthorized",
-    "detailedMessage": "Unauthorized user.",
+    "httpCode": "400",
+    "errorCode": "API-RISKSANALYSIS-400",
+    "message": "Bad Request",
+    "detailedMessage": "ParametroInvalido",
     "link": {
       "rel": "related",
       "href": "https://api.claro.com.br/docs"
     }
   }
 }
-APIGEE = 401</t>
+APIGEE = 400</t>
   </si>
   <si>
     <t>CT002.02 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
@@ -537,25 +537,6 @@
 }
 2 - O response retornado deve apresentar o seguinte valor:
 APIGEE = 400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "403",
-    "errorCode": "API-RISKSANALYSIS-403",
-    "message": "Forbidden",
-    "detailedMessage": "Access denied.",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 403</t>
   </si>
   <si>
     <t>CT002.03 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
@@ -594,25 +575,6 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "404",
-    "errorCode": "API-RISKSANALYSIS-404",
-    "message": "Not found",
-    "detailedMessage": "Resource not found.",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 404</t>
-  </si>
-  <si>
     <t>CT002.04 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
   </si>
   <si>
@@ -649,25 +611,6 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "405",
-    "errorCode": "API-RISKSANALYSIS-405",
-    "message": "Method Not Allowed",
-    "detailedMessage": "Method Not Allowed",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 405</t>
-  </si>
-  <si>
     <t>CT002.05 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
   </si>
   <si>
@@ -702,25 +645,6 @@
 }
 2 - O response retornado deve apresentar o seguinte valor:
 APIGEE = 400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "406",
-    "errorCode": "API-RISKSANALYSIS-406",
-    "message": "Not Acceptable",
-    "detailedMessage": "Not Acceptable",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 406</t>
   </si>
   <si>
     <t>CT002.06 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
@@ -759,25 +683,6 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "415",
-    "errorCode": "API-RISKSANALYSIS-415",
-    "message": "Unsupported Media Type",
-    "detailedMessage": "Unsupported Media Type",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 415</t>
-  </si>
-  <si>
     <t>CT002.07 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
   </si>
   <si>
@@ -814,25 +719,6 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{
-  "apiVersion": "1;2020-06-11",
-  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
-  "error": {
-    "httpCode": "429",
-    "errorCode": "API-RISKSANALYSIS-429",
-    "message": "Too Many Requests",
-    "detailedMessage": "Consumer requests exceeded policies.",
-    "link": {
-      "rel": "related",
-      "href": "https://api.claro.com.br/docs"
-    }
-  }
-}
-APIGEE = 429</t>
-  </si>
-  <si>
     <t>CT002.08 - Request enviada com falha - risksanalysisRequest - Bad Request - COD 400</t>
   </si>
   <si>
@@ -866,12 +752,6 @@
   "zipCode": "02243677"
 }
 2 - O response retornado deve apresentar o seguinte valor:
-APIGEE = 400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Busca apresenta falha.
-2 - Response retorna os seguintes valores:
-{}
 APIGEE = 400</t>
   </si>
   <si>
@@ -1463,6 +1343,25 @@
 APIGEE = 401</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "401",
+    "errorCode": "API-RISKSANALYSIS-401",
+    "message": "Unauthorized",
+    "detailedMessage": "Unauthorized user.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 401</t>
+  </si>
+  <si>
     <t>CT004 - Request enviada com falha - Forbidden - COD 403</t>
   </si>
   <si>
@@ -1482,6 +1381,25 @@
 APIGEE = 403</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "403",
+    "errorCode": "API-RISKSANALYSIS-403",
+    "message": "Forbidden",
+    "detailedMessage": "Access denied.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 403</t>
+  </si>
+  <si>
     <t>CT005 - Request enviada com falha - Not Found - COD 404</t>
   </si>
   <si>
@@ -1501,6 +1419,25 @@
 APIGEE = 404</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "404",
+    "errorCode": "API-RISKSANALYSIS-404",
+    "message": "Not found",
+    "detailedMessage": "Resource not found.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 404</t>
+  </si>
+  <si>
     <t>CT006 - Request enviada com falha - Method Not Allowed - COD 405</t>
   </si>
   <si>
@@ -1520,6 +1457,25 @@
 APIGEE = 405</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "405",
+    "errorCode": "API-RISKSANALYSIS-405",
+    "message": "Method Not Allowed",
+    "detailedMessage": "Method Not Allowed",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 405</t>
+  </si>
+  <si>
     <t>CT007 - Request enviada com falha - Not Acceptable - COD 406</t>
   </si>
   <si>
@@ -1532,6 +1488,25 @@
 APIGEE = 406</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "406",
+    "errorCode": "API-RISKSANALYSIS-406",
+    "message": "Not Acceptable",
+    "detailedMessage": "Not Acceptable",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 406</t>
+  </si>
+  <si>
     <t>CT008 - Request enviada com falha - Unsupported Media Type - COD 415</t>
   </si>
   <si>
@@ -1541,6 +1516,25 @@
     <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
 Content-Type: text/plain
 2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "415",
+    "errorCode": "API-RISKSANALYSIS-415",
+    "message": "Unsupported Media Type",
+    "detailedMessage": "Unsupported Media Type",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
 APIGEE = 415</t>
   </si>
   <si>
@@ -1560,6 +1554,25 @@
 APIGEE = 429</t>
   </si>
   <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2020-06-11",
+  "transactionId": "e6e4e0f4-089d-4194-845e-78f45426f7c7",
+  "error": {
+    "httpCode": "429",
+    "errorCode": "API-RISKSANALYSIS-429",
+    "message": "Too Many Requests",
+    "detailedMessage": "Consumer requests exceeded policies.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 429</t>
+  </si>
+  <si>
     <t>CT001.01 - Request enviada com falha - Bad Request - COD 400</t>
   </si>
   <si>
@@ -1584,6 +1597,12 @@
   "partyIdentificationType": "CPF"
 }
 2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{}
 APIGEE = 400</t>
   </si>
   <si>
@@ -2294,7 +2313,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>20</v>
@@ -2314,25 +2333,25 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>20</v>
@@ -2352,13 +2371,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -2367,10 +2386,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>20</v>
@@ -2390,13 +2409,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -2405,10 +2424,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
@@ -2428,13 +2447,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -2443,10 +2462,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>20</v>
@@ -2466,13 +2485,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
@@ -2481,10 +2500,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>20</v>
@@ -2504,13 +2523,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
@@ -2519,10 +2538,10 @@
         <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>20</v>
@@ -2542,13 +2561,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>16</v>
@@ -2557,10 +2576,10 @@
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>20</v>
@@ -2580,13 +2599,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -2595,10 +2614,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>20</v>
@@ -2618,13 +2637,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
@@ -2633,10 +2652,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>20</v>
@@ -2656,13 +2675,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
@@ -2671,10 +2690,10 @@
         <v>17</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>20</v>
@@ -2694,13 +2713,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>16</v>
@@ -2709,10 +2728,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>20</v>
@@ -2732,13 +2751,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
@@ -2747,10 +2766,10 @@
         <v>17</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>20</v>
@@ -2770,13 +2789,13 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>16</v>
@@ -2785,10 +2804,10 @@
         <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>20</v>
@@ -2808,13 +2827,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>16</v>
@@ -2823,10 +2842,10 @@
         <v>17</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>20</v>
@@ -2846,13 +2865,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>16</v>
@@ -2861,10 +2880,10 @@
         <v>17</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>20</v>
@@ -2884,13 +2903,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
@@ -2899,10 +2918,10 @@
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>20</v>
@@ -2922,13 +2941,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>16</v>
@@ -2937,10 +2956,10 @@
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>20</v>
@@ -2960,13 +2979,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>16</v>
@@ -2975,10 +2994,10 @@
         <v>17</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>20</v>
@@ -2998,13 +3017,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
@@ -3013,10 +3032,10 @@
         <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>20</v>
@@ -3036,13 +3055,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>16</v>
@@ -3051,10 +3070,10 @@
         <v>17</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>20</v>
@@ -3074,13 +3093,13 @@
         <v>12</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>16</v>
@@ -3089,10 +3108,10 @@
         <v>17</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>20</v>
@@ -3112,13 +3131,13 @@
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>16</v>
@@ -3127,10 +3146,10 @@
         <v>17</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>20</v>
@@ -3150,13 +3169,13 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -3165,10 +3184,10 @@
         <v>17</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>20</v>
@@ -3188,13 +3207,13 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3203,10 +3222,10 @@
         <v>17</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>20</v>
@@ -3226,13 +3245,13 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3241,10 +3260,10 @@
         <v>17</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>20</v>
@@ -3264,25 +3283,25 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>20</v>
@@ -3302,13 +3321,13 @@
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3317,10 +3336,10 @@
         <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>20</v>
@@ -3340,25 +3359,25 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>20</v>
@@ -3378,25 +3397,25 @@
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>20</v>
@@ -3494,7 +3513,7 @@
         <v>135</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>20</v>
@@ -3514,25 +3533,25 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
@@ -3552,13 +3571,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -3567,10 +3586,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -3590,13 +3609,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -3605,10 +3624,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>20</v>
@@ -3628,13 +3647,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -3643,10 +3662,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>20</v>
@@ -3666,13 +3685,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -3681,10 +3700,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>20</v>
@@ -3704,13 +3723,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -3719,10 +3738,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
@@ -3742,13 +3761,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -3757,10 +3776,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>20</v>
@@ -3780,13 +3799,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
@@ -3795,10 +3814,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>20</v>
@@ -3818,25 +3837,25 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>20</v>

</xml_diff>